<commit_message>
string mapindex ="Map"+ numeric.GetAsInt(NumericType.LocalMap);出错。现在可以使用角色来完成登录，但是有BUG
</commit_message>
<xml_diff>
--- a/Excel/Numeric.xlsx
+++ b/Excel/Numeric.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView windowHeight="17680"/>
+    <workbookView windowWidth="27945" windowHeight="12255"/>
   </bookViews>
   <sheets>
     <sheet name="Numeric" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="86">
   <si>
     <t>#</t>
   </si>
@@ -279,6 +279,12 @@
   </si>
   <si>
     <t>Hp</t>
+  </si>
+  <si>
+    <t>所在地图</t>
+  </si>
+  <si>
+    <t>LocalMap</t>
   </si>
 </sst>
 </file>
@@ -1285,20 +1291,20 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="B2:J45"/>
+  <dimension ref="B2:J46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I33" sqref="I33"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="O37" sqref="O37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="21.1272727272727" style="2" customWidth="1"/>
-    <col min="2" max="2" width="18.6272727272727" style="2" customWidth="1"/>
-    <col min="3" max="3" width="12.6272727272727" style="3" customWidth="1"/>
+    <col min="1" max="1" width="21.125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="18.625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="12.625" style="3" customWidth="1"/>
     <col min="4" max="4" width="36" style="3" customWidth="1"/>
-    <col min="5" max="5" width="11.6272727272727" style="3" customWidth="1"/>
-    <col min="6" max="10" width="12.2545454545455" style="3" customWidth="1"/>
+    <col min="5" max="5" width="11.625" style="3" customWidth="1"/>
+    <col min="6" max="10" width="12.2583333333333" style="3" customWidth="1"/>
     <col min="11" max="16384" width="9" style="2"/>
   </cols>
   <sheetData>
@@ -1316,7 +1322,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" ht="13.5" spans="3:10">
+    <row r="3" spans="3:10">
       <c r="C3" s="4" t="s">
         <v>2</v>
       </c>
@@ -1340,7 +1346,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" ht="13.5" spans="3:10">
+    <row r="4" spans="3:10">
       <c r="C4" s="4" t="s">
         <v>2</v>
       </c>
@@ -1364,7 +1370,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" ht="13.5" spans="3:10">
+    <row r="5" spans="3:10">
       <c r="C5" s="4" t="s">
         <v>15</v>
       </c>
@@ -1388,7 +1394,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" customFormat="1" ht="14" spans="2:10">
+    <row r="6" customFormat="1" ht="13.5" spans="2:10">
       <c r="B6" s="5" t="s">
         <v>18</v>
       </c>
@@ -1953,7 +1959,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="31" ht="17.5" spans="2:10">
+    <row r="31" ht="18" spans="2:10">
       <c r="B31" s="2" t="s">
         <v>0</v>
       </c>
@@ -2208,6 +2214,32 @@
         <v>111</v>
       </c>
     </row>
+    <row r="46" spans="3:10">
+      <c r="C46" s="3">
+        <v>3009</v>
+      </c>
+      <c r="D46" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="E46" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="F46" s="3">
+        <v>0</v>
+      </c>
+      <c r="G46" s="3">
+        <v>1</v>
+      </c>
+      <c r="H46" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="I46" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="J46" s="3">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>

</xml_diff>